<commit_message>
Automate 15 school seat
</commit_message>
<xml_diff>
--- a/exam_seating_planner/test_seat_plan1.xlsx
+++ b/exam_seating_planner/test_seat_plan1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="78">
   <si>
     <t>Board</t>
   </si>
@@ -94,7 +94,7 @@
     <t>Afternoon</t>
   </si>
   <si>
-    <t>B15</t>
+    <t>A15</t>
   </si>
   <si>
     <t>BD070</t>
@@ -227,6 +227,29 @@
   </si>
   <si>
     <t>F26</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Uttara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mastermind English Medium School, Uttara
+Mastermind English Medium School, Uttara
+</t>
+  </si>
+  <si>
+    <t>Monday, April 24, 2023</t>
+  </si>
+  <si>
+    <t>BD037</t>
+  </si>
+  <si>
+    <t>Mastermind English Medium School, Uttara</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -321,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -374,16 +397,28 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="167" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="167" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="167" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -706,33 +741,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="23" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="23" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="23" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="22" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="22" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="27" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="27" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="28" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="29" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="29" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="27" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="26" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -833,10 +868,10 @@
         <v>25</v>
       </c>
       <c r="J2" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K2" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L2" s="7">
         <v>9095</v>
@@ -902,10 +937,10 @@
         <v>25</v>
       </c>
       <c r="J3" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K3" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L3" s="13">
         <v>9096</v>
@@ -971,10 +1006,10 @@
         <v>25</v>
       </c>
       <c r="J4" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K4" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L4" s="7">
         <v>9097</v>
@@ -1040,10 +1075,10 @@
         <v>25</v>
       </c>
       <c r="J5" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K5" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L5" s="13">
         <v>9099</v>
@@ -1109,10 +1144,10 @@
         <v>25</v>
       </c>
       <c r="J6" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K6" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L6" s="7">
         <v>9101</v>
@@ -1178,10 +1213,10 @@
         <v>25</v>
       </c>
       <c r="J7" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K7" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L7" s="13">
         <v>9104</v>
@@ -1247,10 +1282,10 @@
         <v>25</v>
       </c>
       <c r="J8" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K8" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L8" s="7">
         <v>9105</v>
@@ -1316,10 +1351,10 @@
         <v>25</v>
       </c>
       <c r="J9" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K9" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L9" s="13">
         <v>9107</v>
@@ -1385,10 +1420,10 @@
         <v>25</v>
       </c>
       <c r="J10" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K10" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L10" s="7">
         <v>5001</v>
@@ -1454,10 +1489,10 @@
         <v>25</v>
       </c>
       <c r="J11" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K11" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L11" s="13">
         <v>5026</v>
@@ -1523,10 +1558,10 @@
         <v>25</v>
       </c>
       <c r="J12" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K12" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L12" s="7">
         <v>5027</v>
@@ -1592,10 +1627,10 @@
         <v>25</v>
       </c>
       <c r="J13" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K13" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L13" s="13">
         <v>5028</v>
@@ -1661,10 +1696,10 @@
         <v>25</v>
       </c>
       <c r="J14" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K14" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L14" s="7">
         <v>5029</v>
@@ -1730,10 +1765,10 @@
         <v>25</v>
       </c>
       <c r="J15" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K15" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L15" s="13">
         <v>5031</v>
@@ -1799,10 +1834,10 @@
         <v>25</v>
       </c>
       <c r="J16" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K16" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L16" s="7">
         <v>5032</v>
@@ -1868,10 +1903,10 @@
         <v>25</v>
       </c>
       <c r="J17" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K17" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L17" s="13">
         <v>5033</v>
@@ -1937,10 +1972,10 @@
         <v>25</v>
       </c>
       <c r="J18" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K18" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L18" s="7">
         <v>5034</v>
@@ -2006,10 +2041,10 @@
         <v>25</v>
       </c>
       <c r="J19" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K19" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L19" s="13">
         <v>5035</v>
@@ -2075,10 +2110,10 @@
         <v>25</v>
       </c>
       <c r="J20" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K20" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L20" s="7">
         <v>5037</v>
@@ -2144,10 +2179,10 @@
         <v>25</v>
       </c>
       <c r="J21" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K21" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L21" s="13">
         <v>5038</v>
@@ -2213,10 +2248,10 @@
         <v>25</v>
       </c>
       <c r="J22" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K22" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L22" s="7">
         <v>5039</v>
@@ -2282,10 +2317,10 @@
         <v>25</v>
       </c>
       <c r="J23" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K23" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L23" s="13">
         <v>5040</v>
@@ -2351,10 +2386,10 @@
         <v>25</v>
       </c>
       <c r="J24" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K24" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L24" s="7">
         <v>5041</v>
@@ -2420,10 +2455,10 @@
         <v>25</v>
       </c>
       <c r="J25" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K25" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L25" s="13">
         <v>5042</v>
@@ -2489,10 +2524,10 @@
         <v>25</v>
       </c>
       <c r="J26" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K26" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L26" s="7">
         <v>5044</v>
@@ -2558,10 +2593,10 @@
         <v>25</v>
       </c>
       <c r="J27" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K27" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L27" s="13">
         <v>5046</v>
@@ -2627,10 +2662,10 @@
         <v>25</v>
       </c>
       <c r="J28" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K28" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L28" s="7">
         <v>5047</v>
@@ -2696,10 +2731,10 @@
         <v>25</v>
       </c>
       <c r="J29" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K29" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L29" s="13">
         <v>5048</v>
@@ -2765,10 +2800,10 @@
         <v>25</v>
       </c>
       <c r="J30" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K30" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L30" s="7">
         <v>5049</v>
@@ -2834,10 +2869,10 @@
         <v>25</v>
       </c>
       <c r="J31" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K31" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L31" s="13">
         <v>5050</v>
@@ -2903,10 +2938,10 @@
         <v>25</v>
       </c>
       <c r="J32" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K32" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L32" s="7">
         <v>5051</v>
@@ -2972,10 +3007,10 @@
         <v>25</v>
       </c>
       <c r="J33" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K33" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L33" s="13">
         <v>5053</v>
@@ -3041,10 +3076,10 @@
         <v>25</v>
       </c>
       <c r="J34" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K34" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L34" s="7">
         <v>5054</v>
@@ -3110,10 +3145,10 @@
         <v>25</v>
       </c>
       <c r="J35" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K35" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L35" s="13">
         <v>5055</v>
@@ -3179,10 +3214,10 @@
         <v>25</v>
       </c>
       <c r="J36" s="9">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K36" s="9">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L36" s="7">
         <v>5057</v>
@@ -3248,10 +3283,10 @@
         <v>25</v>
       </c>
       <c r="J37" s="15">
-        <v>5.623842592592593</v>
+        <v>7.623379629629629</v>
       </c>
       <c r="K37" s="15">
-        <v>5.707175925925926</v>
+        <v>7.706712962962963</v>
       </c>
       <c r="L37" s="13">
         <v>5059</v>
@@ -3289,26 +3324,66 @@
       <c r="AA37" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="6"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
+      <c r="A38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="13">
+        <v>320402</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="13">
+        <v>120</v>
+      </c>
+      <c r="G38" s="14">
+        <v>45040</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J38" s="15">
+        <v>45292.623611111114</v>
+      </c>
+      <c r="K38" s="15">
+        <v>45292.70694444444</v>
+      </c>
+      <c r="L38" s="13">
+        <v>5060</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P38" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q38" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R38" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="S38" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T38" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
       <c r="W38" s="6"/>
@@ -3318,26 +3393,66 @@
       <c r="AA38" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="12"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="12"/>
-      <c r="S39" s="12"/>
-      <c r="T39" s="12"/>
+      <c r="A39" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="18">
+        <v>320401</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="18">
+        <v>120</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="19">
+        <v>45292.625</v>
+      </c>
+      <c r="K39" s="19">
+        <v>45292.708333333336</v>
+      </c>
+      <c r="L39" s="18">
+        <v>5487</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P39" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q39" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R39" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="S39" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="U39" s="12"/>
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
@@ -3347,26 +3462,56 @@
       <c r="AA39" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="6"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="6"/>
+      <c r="A40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="21"/>
+      <c r="C40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="P40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="R40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="S40" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="T40" s="20" t="s">
+        <v>77</v>
+      </c>
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
@@ -3376,26 +3521,56 @@
       <c r="AA40" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="12"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="12"/>
-      <c r="S41" s="12"/>
-      <c r="T41" s="12"/>
+      <c r="A41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="18"/>
+      <c r="G41" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="O41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="S41" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="T41" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="U41" s="12"/>
       <c r="V41" s="12"/>
       <c r="W41" s="12"/>
@@ -3405,26 +3580,56 @@
       <c r="AA41" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="6"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="6"/>
+      <c r="A42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="P42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="R42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="S42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="T42" s="20" t="s">
+        <v>77</v>
+      </c>
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
       <c r="W42" s="6"/>
@@ -3434,26 +3639,58 @@
       <c r="AA42" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="12"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="12"/>
-      <c r="S43" s="12"/>
-      <c r="T43" s="12"/>
+      <c r="A43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="M43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="O43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="S43" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="T43" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="U43" s="12"/>
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
@@ -3463,26 +3700,56 @@
       <c r="AA43" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="6"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
+      <c r="A44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="21"/>
+      <c r="C44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="21"/>
+      <c r="G44" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="P44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="R44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="S44" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="T44" s="20" t="s">
+        <v>77</v>
+      </c>
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
@@ -3492,26 +3759,56 @@
       <c r="AA44" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="12"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="12"/>
-      <c r="R45" s="12"/>
-      <c r="S45" s="12"/>
-      <c r="T45" s="12"/>
+      <c r="A45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="O45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="S45" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="T45" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="U45" s="12"/>
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
@@ -3521,26 +3818,56 @@
       <c r="AA45" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="6"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
-      <c r="S46" s="6"/>
-      <c r="T46" s="6"/>
+      <c r="A46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="21"/>
+      <c r="C46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="21"/>
+      <c r="G46" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="P46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="R46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="S46" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="T46" s="20" t="s">
+        <v>77</v>
+      </c>
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
       <c r="W46" s="6"/>
@@ -3549,27 +3876,57 @@
       <c r="Z46" s="6"/>
       <c r="AA46" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="12"/>
-      <c r="Q47" s="12"/>
-      <c r="R47" s="12"/>
-      <c r="S47" s="12"/>
-      <c r="T47" s="12"/>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="18"/>
+      <c r="C47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="18"/>
+      <c r="G47" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="O47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="S47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="T47" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="U47" s="12"/>
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>

</xml_diff>

<commit_message>
Implement the final codebase
</commit_message>
<xml_diff>
--- a/exam_seating_planner/test_seat_plan1.xlsx
+++ b/exam_seating_planner/test_seat_plan1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="77">
   <si>
     <t>Board</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>Mastermind English Medium School, Uttara</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -344,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -400,25 +397,19 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="167" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="167" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="167" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -741,33 +732,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="27" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="27" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="28" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="29" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="29" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="27" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="26" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="27" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="27" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="25" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="24" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -868,10 +859,10 @@
         <v>25</v>
       </c>
       <c r="J2" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K2" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L2" s="7">
         <v>9095</v>
@@ -937,10 +928,10 @@
         <v>25</v>
       </c>
       <c r="J3" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K3" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L3" s="13">
         <v>9096</v>
@@ -1006,10 +997,10 @@
         <v>25</v>
       </c>
       <c r="J4" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K4" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L4" s="7">
         <v>9097</v>
@@ -1075,10 +1066,10 @@
         <v>25</v>
       </c>
       <c r="J5" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K5" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L5" s="13">
         <v>9099</v>
@@ -1144,10 +1135,10 @@
         <v>25</v>
       </c>
       <c r="J6" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K6" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L6" s="7">
         <v>9101</v>
@@ -1213,10 +1204,10 @@
         <v>25</v>
       </c>
       <c r="J7" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K7" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L7" s="13">
         <v>9104</v>
@@ -1282,10 +1273,10 @@
         <v>25</v>
       </c>
       <c r="J8" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K8" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L8" s="7">
         <v>9105</v>
@@ -1351,10 +1342,10 @@
         <v>25</v>
       </c>
       <c r="J9" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K9" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L9" s="13">
         <v>9107</v>
@@ -1420,10 +1411,10 @@
         <v>25</v>
       </c>
       <c r="J10" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K10" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L10" s="7">
         <v>5001</v>
@@ -1489,10 +1480,10 @@
         <v>25</v>
       </c>
       <c r="J11" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K11" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L11" s="13">
         <v>5026</v>
@@ -1558,10 +1549,10 @@
         <v>25</v>
       </c>
       <c r="J12" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K12" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L12" s="7">
         <v>5027</v>
@@ -1627,10 +1618,10 @@
         <v>25</v>
       </c>
       <c r="J13" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K13" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L13" s="13">
         <v>5028</v>
@@ -1696,10 +1687,10 @@
         <v>25</v>
       </c>
       <c r="J14" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K14" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L14" s="7">
         <v>5029</v>
@@ -1765,10 +1756,10 @@
         <v>25</v>
       </c>
       <c r="J15" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K15" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L15" s="13">
         <v>5031</v>
@@ -1834,10 +1825,10 @@
         <v>25</v>
       </c>
       <c r="J16" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K16" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L16" s="7">
         <v>5032</v>
@@ -1903,10 +1894,10 @@
         <v>25</v>
       </c>
       <c r="J17" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K17" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L17" s="13">
         <v>5033</v>
@@ -1972,10 +1963,10 @@
         <v>25</v>
       </c>
       <c r="J18" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K18" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L18" s="7">
         <v>5034</v>
@@ -2041,10 +2032,10 @@
         <v>25</v>
       </c>
       <c r="J19" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K19" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L19" s="13">
         <v>5035</v>
@@ -2110,10 +2101,10 @@
         <v>25</v>
       </c>
       <c r="J20" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K20" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L20" s="7">
         <v>5037</v>
@@ -2179,10 +2170,10 @@
         <v>25</v>
       </c>
       <c r="J21" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K21" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L21" s="13">
         <v>5038</v>
@@ -2248,10 +2239,10 @@
         <v>25</v>
       </c>
       <c r="J22" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K22" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L22" s="7">
         <v>5039</v>
@@ -2317,10 +2308,10 @@
         <v>25</v>
       </c>
       <c r="J23" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K23" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L23" s="13">
         <v>5040</v>
@@ -2386,10 +2377,10 @@
         <v>25</v>
       </c>
       <c r="J24" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K24" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L24" s="7">
         <v>5041</v>
@@ -2455,10 +2446,10 @@
         <v>25</v>
       </c>
       <c r="J25" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K25" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L25" s="13">
         <v>5042</v>
@@ -2524,10 +2515,10 @@
         <v>25</v>
       </c>
       <c r="J26" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K26" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L26" s="7">
         <v>5044</v>
@@ -2593,10 +2584,10 @@
         <v>25</v>
       </c>
       <c r="J27" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K27" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L27" s="13">
         <v>5046</v>
@@ -2662,10 +2653,10 @@
         <v>25</v>
       </c>
       <c r="J28" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K28" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L28" s="7">
         <v>5047</v>
@@ -2731,10 +2722,10 @@
         <v>25</v>
       </c>
       <c r="J29" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K29" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L29" s="13">
         <v>5048</v>
@@ -2800,10 +2791,10 @@
         <v>25</v>
       </c>
       <c r="J30" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K30" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L30" s="7">
         <v>5049</v>
@@ -2869,10 +2860,10 @@
         <v>25</v>
       </c>
       <c r="J31" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K31" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L31" s="13">
         <v>5050</v>
@@ -2938,10 +2929,10 @@
         <v>25</v>
       </c>
       <c r="J32" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K32" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L32" s="7">
         <v>5051</v>
@@ -3007,10 +2998,10 @@
         <v>25</v>
       </c>
       <c r="J33" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K33" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L33" s="13">
         <v>5053</v>
@@ -3076,10 +3067,10 @@
         <v>25</v>
       </c>
       <c r="J34" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K34" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L34" s="7">
         <v>5054</v>
@@ -3145,10 +3136,10 @@
         <v>25</v>
       </c>
       <c r="J35" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K35" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L35" s="13">
         <v>5055</v>
@@ -3214,10 +3205,10 @@
         <v>25</v>
       </c>
       <c r="J36" s="9">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K36" s="9">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L36" s="7">
         <v>5057</v>
@@ -3283,10 +3274,10 @@
         <v>25</v>
       </c>
       <c r="J37" s="15">
-        <v>7.623379629629629</v>
+        <v>8.623148148148148</v>
       </c>
       <c r="K37" s="15">
-        <v>7.706712962962963</v>
+        <v>8.706481481481482</v>
       </c>
       <c r="L37" s="13">
         <v>5059</v>
@@ -3411,7 +3402,7 @@
       <c r="F39" s="18">
         <v>120</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="G39" s="19" t="s">
         <v>74</v>
       </c>
       <c r="H39" s="12" t="s">
@@ -3420,10 +3411,10 @@
       <c r="I39" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J39" s="19">
+      <c r="J39" s="20">
         <v>45292.625</v>
       </c>
-      <c r="K39" s="19">
+      <c r="K39" s="20">
         <v>45292.708333333336</v>
       </c>
       <c r="L39" s="18">
@@ -3462,56 +3453,26 @@
       <c r="AA39" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="A40" s="6"/>
       <c r="B40" s="21"/>
-      <c r="C40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
       <c r="F40" s="21"/>
-      <c r="G40" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="H40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I40" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="G40" s="22"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
       <c r="J40" s="23"/>
       <c r="K40" s="23"/>
       <c r="L40" s="21"/>
-      <c r="M40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="O40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="P40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="R40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="S40" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="T40" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
@@ -3521,56 +3482,26 @@
       <c r="AA40" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="A41" s="12"/>
       <c r="B41" s="18"/>
-      <c r="C41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="18"/>
-      <c r="G41" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
       <c r="L41" s="18"/>
-      <c r="M41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="N41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="P41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="R41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="S41" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="T41" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
       <c r="U41" s="12"/>
       <c r="V41" s="12"/>
       <c r="W41" s="12"/>
@@ -3580,56 +3511,26 @@
       <c r="AA41" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="A42" s="6"/>
       <c r="B42" s="21"/>
-      <c r="C42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
       <c r="F42" s="21"/>
-      <c r="G42" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="H42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I42" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="G42" s="22"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
       <c r="J42" s="23"/>
       <c r="K42" s="23"/>
       <c r="L42" s="21"/>
-      <c r="M42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="O42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="P42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="R42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="S42" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="T42" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
       <c r="W42" s="6"/>
@@ -3639,58 +3540,26 @@
       <c r="AA42" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="A43" s="12"/>
       <c r="B43" s="18"/>
-      <c r="C43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="18"/>
-      <c r="G43" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="M43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="N43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="P43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="R43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="S43" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="T43" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="G43" s="19"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
+      <c r="S43" s="12"/>
+      <c r="T43" s="12"/>
       <c r="U43" s="12"/>
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
@@ -3700,56 +3569,26 @@
       <c r="AA43" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="A44" s="6"/>
       <c r="B44" s="21"/>
-      <c r="C44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
       <c r="F44" s="21"/>
-      <c r="G44" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="H44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I44" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="G44" s="22"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="21"/>
-      <c r="M44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="O44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="P44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="R44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="S44" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="T44" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
@@ -3759,56 +3598,26 @@
       <c r="AA44" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="A45" s="12"/>
       <c r="B45" s="18"/>
-      <c r="C45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
       <c r="L45" s="18"/>
-      <c r="M45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="N45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="P45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="R45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="S45" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="T45" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
       <c r="U45" s="12"/>
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
@@ -3818,56 +3627,26 @@
       <c r="AA45" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="A46" s="6"/>
       <c r="B46" s="21"/>
-      <c r="C46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="21"/>
-      <c r="G46" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="H46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I46" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="G46" s="22"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
       <c r="J46" s="23"/>
       <c r="K46" s="23"/>
       <c r="L46" s="21"/>
-      <c r="M46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="O46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="P46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="R46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="S46" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="T46" s="20" t="s">
-        <v>77</v>
-      </c>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
       <c r="W46" s="6"/>
@@ -3877,56 +3656,26 @@
       <c r="AA46" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="A47" s="12"/>
       <c r="B47" s="18"/>
-      <c r="C47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
       <c r="F47" s="18"/>
-      <c r="G47" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
       <c r="L47" s="18"/>
-      <c r="M47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="N47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="O47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="P47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="R47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="S47" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="T47" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="12"/>
       <c r="U47" s="12"/>
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>

</xml_diff>